<commit_message>
Fixed alignment for header and footer. Fixed spreadsheet view.
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/ss.xlsx
+++ b/src/main/webapp/WEB-INF/books/ss.xlsx
@@ -22,14 +22,6 @@
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" characterSet="UTF-8"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
-  <si>
-    <t>f</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -91,7 +83,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -106,36 +98,7 @@
     <col min="9" max="9" style="1" width="9.142308"/>
     <col min="10" max="16384" style="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="I5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>

</xml_diff>